<commit_message>
Refactor. Fixed error in segment 7 root alignment load
</commit_message>
<xml_diff>
--- a/tabular/core/flu-refseqs.isolates.xlsx
+++ b/tabular/core/flu-refseqs.isolates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/flu/Flu-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF522C2-3B62-2F44-AA26-48DE52A2AA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F022E6EA-2F19-3245-B916-9DD4525CA3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20780" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="756">
   <si>
     <t>strain_id</t>
   </si>
@@ -2243,9 +2243,6 @@
   </si>
   <si>
     <t>Hong Kong</t>
-  </si>
-  <si>
-    <t>ND</t>
   </si>
   <si>
     <t>iav</t>
@@ -3152,8 +3149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="A1:AB61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3254,16 +3251,16 @@
         <v>739</v>
       </c>
       <c r="B2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C2">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>741</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>741</v>
+        <v>45</v>
       </c>
       <c r="F2">
         <v>1973</v>
@@ -3337,16 +3334,16 @@
         <v>728</v>
       </c>
       <c r="B3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C3">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>741</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>741</v>
+        <v>45</v>
       </c>
       <c r="F3">
         <v>1950</v>
@@ -3370,25 +3367,25 @@
         <v>47</v>
       </c>
       <c r="M3" t="s">
+        <v>745</v>
+      </c>
+      <c r="N3" t="s">
         <v>746</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>747</v>
-      </c>
-      <c r="O3" t="s">
-        <v>748</v>
       </c>
       <c r="P3" t="s">
         <v>729</v>
       </c>
       <c r="Q3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="R3" t="s">
         <v>730</v>
       </c>
       <c r="S3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="T3" t="s">
         <v>47</v>
@@ -3423,16 +3420,16 @@
         <v>726</v>
       </c>
       <c r="B4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C4">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>741</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>741</v>
+        <v>45</v>
       </c>
       <c r="F4">
         <v>2011</v>
@@ -3456,25 +3453,25 @@
         <v>47</v>
       </c>
       <c r="M4" t="s">
+        <v>749</v>
+      </c>
+      <c r="N4" t="s">
         <v>750</v>
-      </c>
-      <c r="N4" t="s">
-        <v>751</v>
       </c>
       <c r="O4" t="s">
         <v>727</v>
       </c>
       <c r="P4" t="s">
+        <v>751</v>
+      </c>
+      <c r="Q4" t="s">
         <v>752</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>753</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>754</v>
-      </c>
-      <c r="S4" t="s">
-        <v>755</v>
       </c>
       <c r="T4" t="s">
         <v>47</v>
@@ -3509,7 +3506,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C5">
         <v>198</v>
@@ -3595,7 +3592,7 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C6">
         <v>26</v>
@@ -3681,7 +3678,7 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C7">
         <v>48</v>
@@ -3767,7 +3764,7 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C8">
         <v>58</v>
@@ -3853,7 +3850,7 @@
         <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C9">
         <v>48</v>
@@ -3939,7 +3936,7 @@
         <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C10">
         <v>57</v>
@@ -4025,7 +4022,7 @@
         <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C11">
         <v>66</v>
@@ -4111,7 +4108,7 @@
         <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C12">
         <v>70</v>
@@ -4197,7 +4194,7 @@
         <v>142</v>
       </c>
       <c r="B13" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C13">
         <v>42</v>
@@ -4283,7 +4280,7 @@
         <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C14">
         <v>58</v>
@@ -4369,7 +4366,7 @@
         <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C15">
         <v>66</v>
@@ -4455,7 +4452,7 @@
         <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C16">
         <v>48</v>
@@ -4541,7 +4538,7 @@
         <v>188</v>
       </c>
       <c r="B17" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C17">
         <v>58</v>
@@ -4627,7 +4624,7 @@
         <v>202</v>
       </c>
       <c r="B18" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C18">
         <v>48</v>
@@ -4713,7 +4710,7 @@
         <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -4799,7 +4796,7 @@
         <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C20">
         <v>18</v>
@@ -4885,7 +4882,7 @@
         <v>237</v>
       </c>
       <c r="B21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C21">
         <v>48</v>
@@ -4971,7 +4968,7 @@
         <v>249</v>
       </c>
       <c r="B22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C22">
         <v>18</v>
@@ -5057,7 +5054,7 @@
         <v>261</v>
       </c>
       <c r="B23" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C23">
         <v>48</v>
@@ -5143,7 +5140,7 @@
         <v>275</v>
       </c>
       <c r="B24" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C24">
         <v>56</v>
@@ -5229,7 +5226,7 @@
         <v>287</v>
       </c>
       <c r="B25" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C25">
         <v>18</v>
@@ -5315,7 +5312,7 @@
         <v>298</v>
       </c>
       <c r="B26" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C26">
         <v>18</v>
@@ -5401,7 +5398,7 @@
         <v>310</v>
       </c>
       <c r="B27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C27">
         <v>48</v>
@@ -5487,7 +5484,7 @@
         <v>322</v>
       </c>
       <c r="B28" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C28">
         <v>48</v>
@@ -5573,7 +5570,7 @@
         <v>333</v>
       </c>
       <c r="B29" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C29">
         <v>48</v>
@@ -5659,7 +5656,7 @@
         <v>347</v>
       </c>
       <c r="B30" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C30">
         <v>18</v>
@@ -5745,7 +5742,7 @@
         <v>358</v>
       </c>
       <c r="B31" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C31">
         <v>48</v>
@@ -5831,7 +5828,7 @@
         <v>369</v>
       </c>
       <c r="B32" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C32">
         <v>58</v>
@@ -5917,7 +5914,7 @@
         <v>381</v>
       </c>
       <c r="B33" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C33">
         <v>68</v>
@@ -6003,7 +6000,7 @@
         <v>393</v>
       </c>
       <c r="B34" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C34">
         <v>18</v>
@@ -6089,7 +6086,7 @@
         <v>407</v>
       </c>
       <c r="B35" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C35">
         <v>48</v>
@@ -6175,7 +6172,7 @@
         <v>420</v>
       </c>
       <c r="B36" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C36">
         <v>48</v>
@@ -6261,7 +6258,7 @@
         <v>431</v>
       </c>
       <c r="B37" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C37">
         <v>58</v>
@@ -6347,7 +6344,7 @@
         <v>443</v>
       </c>
       <c r="B38" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C38">
         <v>48</v>
@@ -6433,7 +6430,7 @@
         <v>455</v>
       </c>
       <c r="B39" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C39">
         <v>48</v>
@@ -6519,7 +6516,7 @@
         <v>468</v>
       </c>
       <c r="B40" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C40">
         <v>48</v>
@@ -6605,7 +6602,7 @@
         <v>481</v>
       </c>
       <c r="B41" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C41">
         <v>56</v>
@@ -6691,7 +6688,7 @@
         <v>495</v>
       </c>
       <c r="B42" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C42">
         <v>18</v>
@@ -6777,7 +6774,7 @@
         <v>508</v>
       </c>
       <c r="B43" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C43">
         <v>58</v>
@@ -6863,7 +6860,7 @@
         <v>520</v>
       </c>
       <c r="B44" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C44">
         <v>28</v>
@@ -6949,7 +6946,7 @@
         <v>533</v>
       </c>
       <c r="B45" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C45">
         <v>26</v>
@@ -7035,7 +7032,7 @@
         <v>542</v>
       </c>
       <c r="B46" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C46">
         <v>48</v>
@@ -7121,7 +7118,7 @@
         <v>554</v>
       </c>
       <c r="B47" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C47">
         <v>18</v>
@@ -7207,7 +7204,7 @@
         <v>566</v>
       </c>
       <c r="B48" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C48">
         <v>18</v>
@@ -7293,7 +7290,7 @@
         <v>577</v>
       </c>
       <c r="B49" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -7379,7 +7376,7 @@
         <v>589</v>
       </c>
       <c r="B50" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C50">
         <v>66</v>
@@ -7465,7 +7462,7 @@
         <v>599</v>
       </c>
       <c r="B51" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C51">
         <v>48</v>
@@ -7551,7 +7548,7 @@
         <v>609</v>
       </c>
       <c r="B52" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C52">
         <v>58</v>
@@ -7637,7 +7634,7 @@
         <v>622</v>
       </c>
       <c r="B53" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C53">
         <v>26</v>
@@ -7723,7 +7720,7 @@
         <v>634</v>
       </c>
       <c r="B54" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C54">
         <v>26</v>
@@ -7809,7 +7806,7 @@
         <v>644</v>
       </c>
       <c r="B55" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C55">
         <v>36</v>
@@ -7895,7 +7892,7 @@
         <v>655</v>
       </c>
       <c r="B56" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C56">
         <v>18</v>
@@ -7981,7 +7978,7 @@
         <v>666</v>
       </c>
       <c r="B57" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C57">
         <v>18</v>
@@ -8067,7 +8064,7 @@
         <v>679</v>
       </c>
       <c r="B58" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C58">
         <v>17</v>
@@ -8153,7 +8150,7 @@
         <v>692</v>
       </c>
       <c r="B59" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C59">
         <v>48</v>
@@ -8239,7 +8236,7 @@
         <v>704</v>
       </c>
       <c r="B60" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C60">
         <v>18</v>
@@ -8325,7 +8322,7 @@
         <v>715</v>
       </c>
       <c r="B61" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C61">
         <v>48</v>

</xml_diff>

<commit_message>
Refactor core build - minimise
</commit_message>
<xml_diff>
--- a/tabular/core/flu-refseqs.isolates.xlsx
+++ b/tabular/core/flu-refseqs.isolates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/Flu-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788821D4-72BE-E04E-88C6-3294901E72C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3600EA66-20D7-F644-A3D6-F5C395F3E6CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="500" windowWidth="27920" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3196,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D36" sqref="A1:AB61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Refactor - sorting out IBV reference muddle
</commit_message>
<xml_diff>
--- a/tabular/core/flu-refseqs.isolates.xlsx
+++ b/tabular/core/flu-refseqs.isolates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/Flu-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C570908-9D60-FA40-8356-0D42543C3CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DE9BDF-1F91-EA4F-B3B4-E06843C83F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="500" windowWidth="27920" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3295,8 +3295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:S65"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Refactor - resolving heinous IBV segment 1 versus 2 confusion
</commit_message>
<xml_diff>
--- a/tabular/core/flu-refseqs.isolates.xlsx
+++ b/tabular/core/flu-refseqs.isolates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/Flu-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DE9BDF-1F91-EA4F-B3B4-E06843C83F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF96B1F-8610-0249-9DFF-A2BE1375E94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="500" windowWidth="27920" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3295,8 +3295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6821,10 +6821,10 @@
         <v>728</v>
       </c>
       <c r="L60" s="12" t="s">
+        <v>720</v>
+      </c>
+      <c r="M60" s="12" t="s">
         <v>721</v>
-      </c>
-      <c r="M60" s="12" t="s">
-        <v>720</v>
       </c>
       <c r="N60" s="12" t="s">
         <v>722</v>
@@ -6923,10 +6923,10 @@
         <v>764</v>
       </c>
       <c r="L62" s="12" t="s">
+        <v>756</v>
+      </c>
+      <c r="M62" s="12" t="s">
         <v>755</v>
-      </c>
-      <c r="M62" s="12" t="s">
-        <v>756</v>
       </c>
       <c r="N62" s="12" t="s">
         <v>757</v>
@@ -6974,10 +6974,10 @@
         <v>134</v>
       </c>
       <c r="L63" s="12" t="s">
+        <v>767</v>
+      </c>
+      <c r="M63" s="12" t="s">
         <v>766</v>
-      </c>
-      <c r="M63" s="12" t="s">
-        <v>767</v>
       </c>
       <c r="N63" s="12" t="s">
         <v>768</v>

</xml_diff>

<commit_message>
Refactor - resolving IBV seg1 vs seg2 issues
</commit_message>
<xml_diff>
--- a/tabular/core/flu-refseqs.isolates.xlsx
+++ b/tabular/core/flu-refseqs.isolates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/Flu-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769F357C-B3B9-4947-8DDE-8710367F84EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCF039A-6CBB-C349-8C1E-F67E77DE6D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="500" windowWidth="27920" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3299,7 +3299,7 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="A1:S65"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6824,10 +6824,10 @@
         <v>728</v>
       </c>
       <c r="L60" s="12" t="s">
+        <v>721</v>
+      </c>
+      <c r="M60" s="12" t="s">
         <v>720</v>
-      </c>
-      <c r="M60" s="12" t="s">
-        <v>721</v>
       </c>
       <c r="N60" s="12" t="s">
         <v>722</v>
@@ -6977,10 +6977,10 @@
         <v>134</v>
       </c>
       <c r="L63" s="12" t="s">
+        <v>766</v>
+      </c>
+      <c r="M63" s="12" t="s">
         <v>767</v>
-      </c>
-      <c r="M63" s="12" t="s">
-        <v>766</v>
       </c>
       <c r="N63" s="12" t="s">
         <v>768</v>

</xml_diff>